<commit_message>
psoc robot code and altium files
code finished and continuid working on pcb
</commit_message>
<xml_diff>
--- a/Poort hexwaarde tabel.xlsx
+++ b/Poort hexwaarde tabel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -138,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,13 +146,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -182,12 +194,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -505,15 +522,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:S13"/>
+  <dimension ref="A2:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13:S13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -562,7 +579,7 @@
       </c>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -608,8 +625,13 @@
         <v>5</v>
       </c>
       <c r="S3" s="2"/>
+      <c r="T3" s="5"/>
+      <c r="U3" t="e">
+        <f xml:space="preserve"> not yet implemented in demonstrator</f>
+        <v>#NAME?</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -656,7 +678,7 @@
       </c>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -703,7 +725,7 @@
       </c>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -750,7 +772,7 @@
       </c>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -797,312 +819,284 @@
       </c>
       <c r="S7" s="2"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2" t="s">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="1" t="s">
+      <c r="O8" s="3"/>
+      <c r="P8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2">
+      <c r="Q8" s="4"/>
+      <c r="R8" s="3">
         <v>23</v>
       </c>
-      <c r="S8" s="2"/>
+      <c r="S8" s="3"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2" t="s">
+      <c r="M9" s="3"/>
+      <c r="N9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1" t="s">
+      <c r="O9" s="3"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="3">
         <v>21</v>
       </c>
-      <c r="S9" s="2"/>
+      <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2" t="s">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="2"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="2">
+      <c r="O10" s="3"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="3">
         <v>20</v>
       </c>
-      <c r="S10" s="2"/>
+      <c r="S10" s="3"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="2">
+      <c r="O11" s="3"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="3">
         <v>18</v>
       </c>
-      <c r="S11" s="2"/>
+      <c r="S11" s="3"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2" t="s">
+      <c r="M12" s="3"/>
+      <c r="N12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="2">
+      <c r="O12" s="3"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="3">
         <v>17</v>
       </c>
-      <c r="S12" s="2"/>
+      <c r="S12" s="3"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2" t="s">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="2">
+      <c r="O13" s="3"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="3">
         <v>16</v>
       </c>
-      <c r="S13" s="2"/>
+      <c r="S13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="A13:C13"/>
@@ -1119,8 +1113,36 @@
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>

</xml_diff>